<commit_message>
Replaced "screen" with "page"
</commit_message>
<xml_diff>
--- a/extras/sample-form/Multi-page timed field list.xlsx
+++ b/extras/sample-form/Multi-page timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D11E36-E24F-6C4B-9966-46AF3672B868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A156C59-1576-9B45-97E3-1680DA9331C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="460" windowWidth="26700" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2734,9 +2734,6 @@
     <t>'Chickens have feathers.|Boats have tires.|Six is a number.|Desks can walk.|Dogs lay eggs.|Football is a meal.'</t>
   </si>
   <si>
-    <t>screen1</t>
-  </si>
-  <si>
     <t>field_data1</t>
   </si>
   <si>
@@ -2758,18 +2755,9 @@
     <t>count-items('|', ${field_data1}) - 1</t>
   </si>
   <si>
-    <t>plug-in-metadata(${screen1})</t>
-  </si>
-  <si>
-    <t>screen2</t>
-  </si>
-  <si>
     <t>field_data2</t>
   </si>
   <si>
-    <t>plug-in-metadata(${screen2})</t>
-  </si>
-  <si>
     <t>timeleft2</t>
   </si>
   <si>
@@ -2788,15 +2776,9 @@
     <t>data_ans2</t>
   </si>
   <si>
-    <t>screen3</t>
-  </si>
-  <si>
     <t>field_data3</t>
   </si>
   <si>
-    <t>plug-in-metadata(${screen3})</t>
-  </si>
-  <si>
     <t>timeleft3</t>
   </si>
   <si>
@@ -2936,6 +2918,24 @@
   </si>
   <si>
     <t>custom-auto-return(goback=${goback})</t>
+  </si>
+  <si>
+    <t>page1</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${page1})</t>
+  </si>
+  <si>
+    <t>page2</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${page2})</t>
+  </si>
+  <si>
+    <t>page3</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${page3})</t>
   </si>
 </sst>
 </file>
@@ -6464,10 +6464,10 @@
   <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6663,7 +6663,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="238" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="255" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -6679,7 +6679,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:23" ht="289" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="306" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>42</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>148</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -6780,12 +6780,12 @@
         <v>149</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="N21" s="53" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6793,13 +6793,13 @@
         <v>377</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>408</v>
+        <v>470</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>372</v>
@@ -6810,10 +6810,10 @@
         <v>149</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>416</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -6821,10 +6821,10 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -6832,13 +6832,13 @@
         <v>163</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>400</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -6846,7 +6846,7 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>319</v>
@@ -6857,10 +6857,10 @@
         <v>148</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -6868,7 +6868,7 @@
         <v>164</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -6876,10 +6876,10 @@
         <v>148</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -6887,12 +6887,12 @@
         <v>149</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="N32" s="53" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -6900,12 +6900,12 @@
         <v>148</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="N33" s="53" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -6913,12 +6913,12 @@
         <v>148</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
       <c r="N34" s="53" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6926,13 +6926,13 @@
         <v>377</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>417</v>
+        <v>472</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>372</v>
@@ -6943,10 +6943,10 @@
         <v>149</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>419</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -6954,10 +6954,10 @@
         <v>148</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -6965,13 +6965,13 @@
         <v>163</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>400</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -6979,7 +6979,7 @@
         <v>148</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="N39" s="9" t="s">
         <v>319</v>
@@ -6990,10 +6990,10 @@
         <v>148</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -7001,7 +7001,7 @@
         <v>164</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -7009,10 +7009,10 @@
         <v>148</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -7020,12 +7020,12 @@
         <v>149</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="N44" s="53" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -7033,12 +7033,12 @@
         <v>148</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="N45" s="53" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -7046,12 +7046,12 @@
         <v>148</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="N46" s="53" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -7059,13 +7059,13 @@
         <v>377</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>426</v>
+        <v>474</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>372</v>
@@ -7076,10 +7076,10 @@
         <v>149</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>428</v>
+        <v>475</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -7087,10 +7087,10 @@
         <v>148</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -7098,13 +7098,13 @@
         <v>163</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>400</v>
       </c>
       <c r="O50" s="9" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -7112,7 +7112,7 @@
         <v>148</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="N51" s="9" t="s">
         <v>319</v>
@@ -7123,10 +7123,10 @@
         <v>148</v>
       </c>
       <c r="B52" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="N52" s="9" t="s">
         <v>434</v>
-      </c>
-      <c r="N52" s="9" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -7134,7 +7134,7 @@
         <v>164</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
@@ -7142,10 +7142,10 @@
         <v>148</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="N54" s="9" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
@@ -7153,12 +7153,12 @@
         <v>149</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="N56" s="53" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
@@ -7166,12 +7166,12 @@
         <v>148</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="N57" s="53" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -7179,12 +7179,12 @@
         <v>148</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="N58" s="53" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -7192,10 +7192,10 @@
         <v>148</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="N59" s="9" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
@@ -7206,7 +7206,7 @@
         <v>380</v>
       </c>
       <c r="N61" s="9" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
@@ -7228,7 +7228,7 @@
         <v>386</v>
       </c>
       <c r="N63" s="9" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -7264,7 +7264,7 @@
         <v>387</v>
       </c>
       <c r="N66" s="9" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -7275,7 +7275,7 @@
         <v>388</v>
       </c>
       <c r="N67" s="9" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -7319,7 +7319,7 @@
         <v>394</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -8333,7 +8333,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007222110</v>
+        <v>2007232029</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>369</v>
@@ -8925,7 +8925,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Updated so no longer needs auto-return field plug-in
</commit_message>
<xml_diff>
--- a/extras/sample-form/Multi-page timed field list.xlsx
+++ b/extras/sample-form/Multi-page timed field list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A156C59-1576-9B45-97E3-1680DA9331C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E854BB9-EEB4-FE48-B1E0-C9F889CAA814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="26700" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="26700" windowHeight="14800" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="469">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2887,39 +2887,6 @@
     <t>item-at('|', ${all_ans}, ${ans_index} - 1)</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${list1}, duration=${time_start}, immediate=1)</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${list2}, duration=${timeleft2}, immediate=1)</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${list3}, duration=${timeleft3}, immediate=1)</t>
-  </si>
-  <si>
-    <t>current_dec_final</t>
-  </si>
-  <si>
-    <t>seconds_past_final</t>
-  </si>
-  <si>
-    <t>(${current_dec_final} - ${dec_start_time}) * 86400</t>
-  </si>
-  <si>
-    <t>timeleft_final</t>
-  </si>
-  <si>
-    <t>${time_start} - ${seconds_past_final}</t>
-  </si>
-  <si>
-    <t>goback</t>
-  </si>
-  <si>
-    <t>if(${timeleft_final} &lt;= 0, 0, 1)</t>
-  </si>
-  <si>
-    <t>custom-auto-return(goback=${goback})</t>
-  </si>
-  <si>
     <t>page1</t>
   </si>
   <si>
@@ -2936,6 +2903,18 @@
   </si>
   <si>
     <t>plug-in-metadata(${page3})</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${list3}, duration=${timeleft3}, endearly=0)</t>
+  </si>
+  <si>
+    <t>This is the last page. There is still time left.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${list2}, duration=${timeleft2})</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${list1}, duration=${time_start})</t>
   </si>
 </sst>
 </file>
@@ -3654,7 +3633,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="310">
+  <dxfs count="275">
     <dxf>
       <fill>
         <patternFill>
@@ -4425,276 +4404,6 @@
           <color auto="1"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6461,13 +6170,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:W65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6663,7 +6372,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="255" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -6679,7 +6388,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:23" ht="306" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="289" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>42</v>
       </c>
@@ -6793,13 +6502,13 @@
         <v>377</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>442</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>372</v>
@@ -6813,7 +6522,7 @@
         <v>408</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -6882,17 +6591,30 @@
         <v>436</v>
       </c>
     </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="N31" s="53" t="s">
+        <v>447</v>
+      </c>
+    </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="N32" s="53" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -6900,78 +6622,76 @@
         <v>148</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>450</v>
+        <v>416</v>
       </c>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="N33" s="53" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>148</v>
+        <v>377</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="N34" s="53" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+        <v>461</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>377</v>
+        <v>149</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>460</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>372</v>
+        <v>415</v>
+      </c>
+      <c r="N35" s="9" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="O37" s="9" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>417</v>
-      </c>
-      <c r="N37" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>163</v>
-      </c>
       <c r="B38" s="9" t="s">
-        <v>418</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -6979,53 +6699,55 @@
         <v>148</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>319</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="N40" s="9" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B42" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="N42" s="9" t="s">
+      <c r="N41" s="9" t="s">
         <v>438</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="N43" s="53" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="N44" s="53" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -7033,78 +6755,79 @@
         <v>148</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>454</v>
+        <v>423</v>
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="N45" s="53" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>148</v>
+        <v>377</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="N46" s="53" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+        <v>463</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>377</v>
+        <v>149</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>461</v>
-      </c>
-      <c r="K47" s="9" t="s">
-        <v>372</v>
+        <v>422</v>
+      </c>
+      <c r="N47" s="9" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="O49" s="9" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="N49" s="9" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
-        <v>163</v>
-      </c>
       <c r="B50" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="O50" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
+      </c>
+      <c r="N50" s="9" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -7112,53 +6835,51 @@
         <v>148</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>319</v>
+        <v>434</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="N52" s="9" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="N53" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>439</v>
-      </c>
-      <c r="N54" s="9" t="s">
-        <v>440</v>
+      <c r="B55" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="N55" s="9" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="N56" s="53" t="s">
-        <v>447</v>
+        <v>381</v>
+      </c>
+      <c r="N56" s="9" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
@@ -7166,25 +6887,24 @@
         <v>148</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="N57" s="53" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+      <c r="N57" s="9" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="N58" s="53" t="s">
-        <v>466</v>
+        <v>385</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="O58" s="9" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -7192,10 +6912,21 @@
         <v>148</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>467</v>
+        <v>384</v>
       </c>
       <c r="N59" s="9" t="s">
-        <v>468</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="N60" s="9" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
@@ -7203,10 +6934,10 @@
         <v>148</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="N61" s="9" t="s">
-        <v>431</v>
+        <v>458</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
@@ -7214,925 +6945,718 @@
         <v>148</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="N62" s="9" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="N63" s="9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
-        <v>163</v>
-      </c>
       <c r="B64" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="O64" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+      <c r="N64" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="N65" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A66" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="N66" s="9" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A67" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="N67" s="9" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="N68" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="N70" s="9" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B71" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C65" s="10" t="s">
         <v>394</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>469</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I43 B43:C43 F43 F35:F41 B35:C41 I35:I41 F47:F53 B47:C53 I47:I53 I1:I31 B1:C31 F1:F31 I55 B55:C55 F55 F59:F1048576 B59:C1048576 I59:I1048576">
-    <cfRule type="expression" dxfId="309" priority="399" stopIfTrue="1">
+  <conditionalFormatting sqref="I42 B42:C42 F42 F34:F40 B34:C40 I34:I40 F46:F52 B46:C52 I46:I52 I1:I30 B1:C30 F1:F30 I54:I1048576 B54:C1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="274" priority="399" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43 B43:C43 O43 O35:O41 B35:C41 I35:I41 O47:O53 B47:C53 I47:I53 I1:I31 B1:C31 O1:O31 I55 B55:C55 O55:O1048576 B59:C1048576 I59:I1048576">
-    <cfRule type="expression" dxfId="308" priority="396" stopIfTrue="1">
+  <conditionalFormatting sqref="I42 B42:C42 O42 O34:O40 B34:C40 I34:I40 O46:O52 B46:C52 I46:I52 I1:I30 B1:C30 O1:O30 O54:O1048576 I54:I1048576 B54:C1048576">
+    <cfRule type="expression" dxfId="273" priority="396" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:D43 F43 F35:F41 B35:D41 F47:F53 B47:D53 B1:D31 F1:F31 B55:D55 F55 F59:F1048576 B59:D1048576">
-    <cfRule type="expression" dxfId="307" priority="393" stopIfTrue="1">
+  <conditionalFormatting sqref="B42:D42 F42 F34:F40 B34:D40 F46:F52 B46:D52 B1:D30 F1:F30 B54:D1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="272" priority="393" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43:H43 B43:D43 B35:D41 G35:H41 B47:D53 G47:H53 G1:H31 B1:D31 G55:H55 B55:D55 B59:D1048576 G59:H1048576">
-    <cfRule type="expression" dxfId="306" priority="391" stopIfTrue="1">
+  <conditionalFormatting sqref="G42:H42 B42:D42 B34:D40 G34:H40 B46:D52 G46:H52 G1:H30 B1:D30 G54:H1048576 B54:D1048576">
+    <cfRule type="expression" dxfId="271" priority="391" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43:H43 B43:D43 B35:D41 G35:H41 B47:D53 G47:H53 G1:H31 B1:D31 G55:H55 B55:D55 B59:D1048576 G59:H1048576">
-    <cfRule type="expression" dxfId="305" priority="389" stopIfTrue="1">
+  <conditionalFormatting sqref="G42:H42 B42:D42 B34:D40 G34:H40 B46:D52 G46:H52 G1:H30 B1:D30 G54:H1048576 B54:D1048576">
+    <cfRule type="expression" dxfId="270" priority="389" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:C43 F43 F35:F41 B35:C41 F47:F53 B47:C53 B1:C31 F1:F31 B55:C55 F55 F59:F1048576 B59:C1048576">
-    <cfRule type="expression" dxfId="304" priority="384" stopIfTrue="1">
+  <conditionalFormatting sqref="B42:C42 F42 F34:F40 B34:C40 F46:F52 B46:C52 B1:C30 F1:F30 B54:C1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="269" priority="384" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 F43 F35:F41 B35:B41 F47:F53 B47:B53 B1:B31 F1:F31 B55 F55 F59:F1048576 B59:B1048576">
-    <cfRule type="expression" dxfId="303" priority="374" stopIfTrue="1">
+  <conditionalFormatting sqref="B42 F42 F34:F40 B34:B40 F46:F52 B46:B52 B1:B30 F1:F30 B54:B1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="268" priority="374" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:C43 B35:C41 B47:C53 B1:C31 B55:C55 B59:C1048576">
-    <cfRule type="expression" dxfId="302" priority="368" stopIfTrue="1">
+  <conditionalFormatting sqref="B42:C42 B34:C40 B46:C52 B1:C30 B54:C1048576">
+    <cfRule type="expression" dxfId="267" priority="368" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="301" priority="370" stopIfTrue="1">
+    <cfRule type="expression" dxfId="266" priority="370" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="372" stopIfTrue="1">
+    <cfRule type="expression" dxfId="265" priority="372" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 N43 N35:N41 B35:B41 N47:N53 B47:B53 B1:B31 N1:N31 B55 N55 N59:N1048576 B59:B1048576">
-    <cfRule type="expression" dxfId="299" priority="366" stopIfTrue="1">
+  <conditionalFormatting sqref="B42 N42 N34:N40 B34:B40 N46:N52 B46:B52 B1:B30 N1:N30 B54:B1048576 N54:N1048576">
+    <cfRule type="expression" dxfId="264" priority="366" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:C43 F43 F35:F41 B35:C41 F47:F53 B47:C53 B1:C31 F1:F31 B55:C55 F55 F59:F1048576 B59:C1048576">
-    <cfRule type="expression" dxfId="298" priority="364" stopIfTrue="1">
+  <conditionalFormatting sqref="B42:C42 F42 F34:F40 B34:C40 F46:F52 B46:C52 B1:C30 F1:F30 B54:C1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="263" priority="364" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:C43 F43 F35:F41 B35:C41 F47:F53 B47:C53 B1:C31 F1:F31 B55:C55 F55 F59:F1048576 B59:C1048576">
-    <cfRule type="expression" dxfId="297" priority="360" stopIfTrue="1">
+  <conditionalFormatting sqref="B42:C42 F42 F34:F40 B34:C40 F46:F52 B46:C52 B1:C30 F1:F30 B54:C1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="262" priority="360" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:C43 B35:C41 B47:C53 B1:C31 B55:C55 B59:C1048576">
-    <cfRule type="expression" dxfId="296" priority="358" stopIfTrue="1">
+  <conditionalFormatting sqref="B42:C42 B34:C40 B46:C52 B1:C30 B54:C1048576">
+    <cfRule type="expression" dxfId="261" priority="358" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:W43 A35:W41 A47:W53 A1:W31 A56:A58 O56:W58 A55:W55 A59:W1048576">
-    <cfRule type="expression" dxfId="295" priority="352" stopIfTrue="1">
+  <conditionalFormatting sqref="A42:W42 A34:W40 A46:W52 A1:W30 A54:W1048576">
+    <cfRule type="expression" dxfId="260" priority="352" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="355" stopIfTrue="1">
+    <cfRule type="expression" dxfId="259" priority="355" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="293" priority="359" stopIfTrue="1">
+    <cfRule type="expression" dxfId="258" priority="359" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="292" priority="361" stopIfTrue="1">
+    <cfRule type="expression" dxfId="257" priority="361" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="365" stopIfTrue="1">
+    <cfRule type="expression" dxfId="256" priority="365" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="367" stopIfTrue="1">
+    <cfRule type="expression" dxfId="255" priority="367" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="289" priority="369" stopIfTrue="1">
+    <cfRule type="expression" dxfId="254" priority="369" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="371" stopIfTrue="1">
+    <cfRule type="expression" dxfId="253" priority="371" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="287" priority="373" stopIfTrue="1">
+    <cfRule type="expression" dxfId="252" priority="373" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="375" stopIfTrue="1">
+    <cfRule type="expression" dxfId="251" priority="375" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="378" stopIfTrue="1">
+    <cfRule type="expression" dxfId="250" priority="378" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="385" stopIfTrue="1">
+    <cfRule type="expression" dxfId="249" priority="385" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="390" stopIfTrue="1">
+    <cfRule type="expression" dxfId="248" priority="390" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="392" stopIfTrue="1">
+    <cfRule type="expression" dxfId="247" priority="392" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="394" stopIfTrue="1">
+    <cfRule type="expression" dxfId="246" priority="394" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="395" stopIfTrue="1">
+    <cfRule type="expression" dxfId="245" priority="395" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="279" priority="397" stopIfTrue="1">
+    <cfRule type="expression" dxfId="244" priority="397" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="398" stopIfTrue="1">
+    <cfRule type="expression" dxfId="243" priority="398" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="277" priority="400" stopIfTrue="1">
+    <cfRule type="expression" dxfId="242" priority="400" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 B35:B41 B47:B53 B1:B31 B55 B59:B1048576">
-    <cfRule type="expression" dxfId="276" priority="353" stopIfTrue="1">
+  <conditionalFormatting sqref="B42 B34:B40 B46:B52 B1:B30 B54:B1048576">
+    <cfRule type="expression" dxfId="241" priority="353" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 F43 F35:F41 B35:B41 F47:F53 B47:B53 B1:B31 F1:F31 B55 F55 F59:F1048576 B59:B1048576">
-    <cfRule type="expression" dxfId="275" priority="351" stopIfTrue="1">
+  <conditionalFormatting sqref="B42 F42 F34:F40 B34:B40 F46:F52 B46:B52 B1:B30 F1:F30 B54:B1048576 F54:F1048576">
+    <cfRule type="expression" dxfId="240" priority="351" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42 B42:C42 F42">
-    <cfRule type="expression" dxfId="274" priority="174" stopIfTrue="1">
-      <formula>$A42="begin group"</formula>
+  <conditionalFormatting sqref="I41 B41:C41 F41">
+    <cfRule type="expression" dxfId="239" priority="174" stopIfTrue="1">
+      <formula>$A41="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42 B42:C42 O42">
-    <cfRule type="expression" dxfId="273" priority="171" stopIfTrue="1">
-      <formula>$A42="begin repeat"</formula>
+  <conditionalFormatting sqref="I41 B41:C41 O41">
+    <cfRule type="expression" dxfId="238" priority="171" stopIfTrue="1">
+      <formula>$A41="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:D42 F42">
-    <cfRule type="expression" dxfId="272" priority="168" stopIfTrue="1">
-      <formula>$A42="text"</formula>
+  <conditionalFormatting sqref="B41:D41 F41">
+    <cfRule type="expression" dxfId="237" priority="168" stopIfTrue="1">
+      <formula>$A41="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42:H42 B42:D42">
-    <cfRule type="expression" dxfId="271" priority="166" stopIfTrue="1">
-      <formula>$A42="integer"</formula>
+  <conditionalFormatting sqref="G41:H41 B41:D41">
+    <cfRule type="expression" dxfId="236" priority="166" stopIfTrue="1">
+      <formula>$A41="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42:H42 B42:D42">
-    <cfRule type="expression" dxfId="270" priority="164" stopIfTrue="1">
-      <formula>$A42="decimal"</formula>
+  <conditionalFormatting sqref="G41:H41 B41:D41">
+    <cfRule type="expression" dxfId="235" priority="164" stopIfTrue="1">
+      <formula>$A41="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:C42 F42">
-    <cfRule type="expression" dxfId="269" priority="162" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A42, 16)="select_multiple ", LEN($A42)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A42, 17)))), AND(LEFT($A42, 11)="select_one ", LEN($A42)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A42, 12)))))</formula>
+  <conditionalFormatting sqref="B41:C41 F41">
+    <cfRule type="expression" dxfId="234" priority="162" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A41, 16)="select_multiple ", LEN($A41)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A41, 17)))), AND(LEFT($A41, 11)="select_one ", LEN($A41)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A41, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42 F42">
-    <cfRule type="expression" dxfId="268" priority="159" stopIfTrue="1">
-      <formula>OR($A42="audio audit", $A42="text audit", $A42="speed violations count", $A42="speed violations list", $A42="speed violations audit")</formula>
+  <conditionalFormatting sqref="B41 F41">
+    <cfRule type="expression" dxfId="233" priority="159" stopIfTrue="1">
+      <formula>OR($A41="audio audit", $A41="text audit", $A41="speed violations count", $A41="speed violations list", $A41="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:C42">
-    <cfRule type="expression" dxfId="267" priority="153" stopIfTrue="1">
-      <formula>$A42="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="266" priority="155" stopIfTrue="1">
-      <formula>$A42="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="265" priority="157" stopIfTrue="1">
-      <formula>OR($A42="geopoint", $A42="geoshape", $A42="geotrace")</formula>
+  <conditionalFormatting sqref="B41:C41">
+    <cfRule type="expression" dxfId="232" priority="153" stopIfTrue="1">
+      <formula>$A41="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="231" priority="155" stopIfTrue="1">
+      <formula>$A41="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="230" priority="157" stopIfTrue="1">
+      <formula>OR($A41="geopoint", $A41="geoshape", $A41="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42 N42">
-    <cfRule type="expression" dxfId="264" priority="151" stopIfTrue="1">
-      <formula>OR($A42="calculate", $A42="calculate_here")</formula>
+  <conditionalFormatting sqref="B41 N41">
+    <cfRule type="expression" dxfId="229" priority="151" stopIfTrue="1">
+      <formula>OR($A41="calculate", $A41="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:C42 F42">
-    <cfRule type="expression" dxfId="263" priority="149" stopIfTrue="1">
-      <formula>OR($A42="date", $A42="datetime")</formula>
+  <conditionalFormatting sqref="B41:C41 F41">
+    <cfRule type="expression" dxfId="228" priority="149" stopIfTrue="1">
+      <formula>OR($A41="date", $A41="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:C42 F42">
-    <cfRule type="expression" dxfId="262" priority="147" stopIfTrue="1">
-      <formula>$A42="image"</formula>
+  <conditionalFormatting sqref="B41:C41 F41">
+    <cfRule type="expression" dxfId="227" priority="147" stopIfTrue="1">
+      <formula>$A41="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:C42">
-    <cfRule type="expression" dxfId="261" priority="145" stopIfTrue="1">
-      <formula>OR($A42="audio", $A42="video")</formula>
+  <conditionalFormatting sqref="B41:C41">
+    <cfRule type="expression" dxfId="226" priority="145" stopIfTrue="1">
+      <formula>OR($A41="audio", $A41="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42:W42">
-    <cfRule type="expression" dxfId="260" priority="142" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A42, 14)="sensor_stream ", LEN($A42)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A42, 15)))), AND(LEFT($A42, 17)="sensor_statistic ", LEN($A42)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A42, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="259" priority="144" stopIfTrue="1">
-      <formula>$A42="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="258" priority="146" stopIfTrue="1">
-      <formula>OR($A42="audio", $A42="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="257" priority="148" stopIfTrue="1">
-      <formula>$A42="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="256" priority="150" stopIfTrue="1">
-      <formula>OR($A42="date", $A42="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="255" priority="152" stopIfTrue="1">
-      <formula>OR($A42="calculate", $A42="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="254" priority="154" stopIfTrue="1">
-      <formula>$A42="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="253" priority="156" stopIfTrue="1">
-      <formula>$A42="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="252" priority="158" stopIfTrue="1">
-      <formula>OR($A42="geopoint", $A42="geoshape", $A42="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="251" priority="160" stopIfTrue="1">
-      <formula>OR($A42="audio audit", $A42="text audit", $A42="speed violations count", $A42="speed violations list", $A42="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="250" priority="161" stopIfTrue="1">
-      <formula>OR($A42="username", $A42="phonenumber", $A42="start", $A42="end", $A42="deviceid", $A42="subscriberid", $A42="simserial", $A42="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="249" priority="163" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A42, 16)="select_multiple ", LEN($A42)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A42, 17)))), AND(LEFT($A42, 11)="select_one ", LEN($A42)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A42, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="248" priority="165" stopIfTrue="1">
-      <formula>$A42="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="247" priority="167" stopIfTrue="1">
-      <formula>$A42="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="246" priority="169" stopIfTrue="1">
-      <formula>$A42="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="245" priority="170" stopIfTrue="1">
-      <formula>$A42="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="244" priority="172" stopIfTrue="1">
-      <formula>$A42="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="243" priority="173" stopIfTrue="1">
-      <formula>$A42="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="242" priority="175" stopIfTrue="1">
-      <formula>$A42="begin group"</formula>
+  <conditionalFormatting sqref="A41:W41">
+    <cfRule type="expression" dxfId="225" priority="142" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A41, 14)="sensor_stream ", LEN($A41)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A41, 15)))), AND(LEFT($A41, 17)="sensor_statistic ", LEN($A41)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A41, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="224" priority="144" stopIfTrue="1">
+      <formula>$A41="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="223" priority="146" stopIfTrue="1">
+      <formula>OR($A41="audio", $A41="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="222" priority="148" stopIfTrue="1">
+      <formula>$A41="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="221" priority="150" stopIfTrue="1">
+      <formula>OR($A41="date", $A41="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="220" priority="152" stopIfTrue="1">
+      <formula>OR($A41="calculate", $A41="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="219" priority="154" stopIfTrue="1">
+      <formula>$A41="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="218" priority="156" stopIfTrue="1">
+      <formula>$A41="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="217" priority="158" stopIfTrue="1">
+      <formula>OR($A41="geopoint", $A41="geoshape", $A41="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="216" priority="160" stopIfTrue="1">
+      <formula>OR($A41="audio audit", $A41="text audit", $A41="speed violations count", $A41="speed violations list", $A41="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="215" priority="161" stopIfTrue="1">
+      <formula>OR($A41="username", $A41="phonenumber", $A41="start", $A41="end", $A41="deviceid", $A41="subscriberid", $A41="simserial", $A41="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="214" priority="163" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A41, 16)="select_multiple ", LEN($A41)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A41, 17)))), AND(LEFT($A41, 11)="select_one ", LEN($A41)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A41, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="213" priority="165" stopIfTrue="1">
+      <formula>$A41="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="212" priority="167" stopIfTrue="1">
+      <formula>$A41="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="211" priority="169" stopIfTrue="1">
+      <formula>$A41="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="210" priority="170" stopIfTrue="1">
+      <formula>$A41="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="209" priority="172" stopIfTrue="1">
+      <formula>$A41="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="208" priority="173" stopIfTrue="1">
+      <formula>$A41="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="207" priority="175" stopIfTrue="1">
+      <formula>$A41="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="241" priority="143" stopIfTrue="1">
-      <formula>$A42="comments"</formula>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" dxfId="206" priority="143" stopIfTrue="1">
+      <formula>$A41="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42 F42">
-    <cfRule type="expression" dxfId="240" priority="141" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A42, 14)="sensor_stream ", LEN($A42)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A42, 15)))), AND(LEFT($A42, 17)="sensor_statistic ", LEN($A42)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A42, 18)))))</formula>
+  <conditionalFormatting sqref="B41 F41">
+    <cfRule type="expression" dxfId="205" priority="141" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A41, 14)="sensor_stream ", LEN($A41)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A41, 15)))), AND(LEFT($A41, 17)="sensor_statistic ", LEN($A41)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A41, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I54 B54:C54 F54">
-    <cfRule type="expression" dxfId="239" priority="139" stopIfTrue="1">
-      <formula>$A54="begin group"</formula>
+  <conditionalFormatting sqref="I53 B53:C53 F53">
+    <cfRule type="expression" dxfId="204" priority="139" stopIfTrue="1">
+      <formula>$A53="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I54 B54:C54 O54">
-    <cfRule type="expression" dxfId="238" priority="136" stopIfTrue="1">
-      <formula>$A54="begin repeat"</formula>
+  <conditionalFormatting sqref="I53 B53:C53 O53">
+    <cfRule type="expression" dxfId="203" priority="136" stopIfTrue="1">
+      <formula>$A53="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:D54 F54">
-    <cfRule type="expression" dxfId="237" priority="133" stopIfTrue="1">
-      <formula>$A54="text"</formula>
+  <conditionalFormatting sqref="B53:D53 F53">
+    <cfRule type="expression" dxfId="202" priority="133" stopIfTrue="1">
+      <formula>$A53="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G54:H54 B54:D54">
-    <cfRule type="expression" dxfId="236" priority="131" stopIfTrue="1">
-      <formula>$A54="integer"</formula>
+  <conditionalFormatting sqref="G53:H53 B53:D53">
+    <cfRule type="expression" dxfId="201" priority="131" stopIfTrue="1">
+      <formula>$A53="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G54:H54 B54:D54">
-    <cfRule type="expression" dxfId="235" priority="129" stopIfTrue="1">
-      <formula>$A54="decimal"</formula>
+  <conditionalFormatting sqref="G53:H53 B53:D53">
+    <cfRule type="expression" dxfId="200" priority="129" stopIfTrue="1">
+      <formula>$A53="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:C54 F54">
-    <cfRule type="expression" dxfId="234" priority="127" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A54, 16)="select_multiple ", LEN($A54)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A54, 17)))), AND(LEFT($A54, 11)="select_one ", LEN($A54)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A54, 12)))))</formula>
+  <conditionalFormatting sqref="B53:C53 F53">
+    <cfRule type="expression" dxfId="199" priority="127" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A53, 16)="select_multiple ", LEN($A53)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A53, 17)))), AND(LEFT($A53, 11)="select_one ", LEN($A53)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A53, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54 F54">
-    <cfRule type="expression" dxfId="233" priority="124" stopIfTrue="1">
-      <formula>OR($A54="audio audit", $A54="text audit", $A54="speed violations count", $A54="speed violations list", $A54="speed violations audit")</formula>
+  <conditionalFormatting sqref="B53 F53">
+    <cfRule type="expression" dxfId="198" priority="124" stopIfTrue="1">
+      <formula>OR($A53="audio audit", $A53="text audit", $A53="speed violations count", $A53="speed violations list", $A53="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:C54">
-    <cfRule type="expression" dxfId="232" priority="118" stopIfTrue="1">
-      <formula>$A54="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="231" priority="120" stopIfTrue="1">
-      <formula>$A54="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="230" priority="122" stopIfTrue="1">
-      <formula>OR($A54="geopoint", $A54="geoshape", $A54="geotrace")</formula>
+  <conditionalFormatting sqref="B53:C53">
+    <cfRule type="expression" dxfId="197" priority="118" stopIfTrue="1">
+      <formula>$A53="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="196" priority="120" stopIfTrue="1">
+      <formula>$A53="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="195" priority="122" stopIfTrue="1">
+      <formula>OR($A53="geopoint", $A53="geoshape", $A53="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54 N54">
-    <cfRule type="expression" dxfId="229" priority="116" stopIfTrue="1">
-      <formula>OR($A54="calculate", $A54="calculate_here")</formula>
+  <conditionalFormatting sqref="B53 N53">
+    <cfRule type="expression" dxfId="194" priority="116" stopIfTrue="1">
+      <formula>OR($A53="calculate", $A53="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:C54 F54">
-    <cfRule type="expression" dxfId="228" priority="114" stopIfTrue="1">
-      <formula>OR($A54="date", $A54="datetime")</formula>
+  <conditionalFormatting sqref="B53:C53 F53">
+    <cfRule type="expression" dxfId="193" priority="114" stopIfTrue="1">
+      <formula>OR($A53="date", $A53="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:C54 F54">
-    <cfRule type="expression" dxfId="227" priority="112" stopIfTrue="1">
-      <formula>$A54="image"</formula>
+  <conditionalFormatting sqref="B53:C53 F53">
+    <cfRule type="expression" dxfId="192" priority="112" stopIfTrue="1">
+      <formula>$A53="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:C54">
-    <cfRule type="expression" dxfId="226" priority="110" stopIfTrue="1">
-      <formula>OR($A54="audio", $A54="video")</formula>
+  <conditionalFormatting sqref="B53:C53">
+    <cfRule type="expression" dxfId="191" priority="110" stopIfTrue="1">
+      <formula>OR($A53="audio", $A53="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54:W54">
-    <cfRule type="expression" dxfId="225" priority="107" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A54, 14)="sensor_stream ", LEN($A54)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A54, 15)))), AND(LEFT($A54, 17)="sensor_statistic ", LEN($A54)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A54, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="224" priority="109" stopIfTrue="1">
-      <formula>$A54="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="223" priority="111" stopIfTrue="1">
-      <formula>OR($A54="audio", $A54="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="222" priority="113" stopIfTrue="1">
-      <formula>$A54="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="221" priority="115" stopIfTrue="1">
-      <formula>OR($A54="date", $A54="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="220" priority="117" stopIfTrue="1">
-      <formula>OR($A54="calculate", $A54="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="219" priority="119" stopIfTrue="1">
-      <formula>$A54="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="218" priority="121" stopIfTrue="1">
-      <formula>$A54="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="217" priority="123" stopIfTrue="1">
-      <formula>OR($A54="geopoint", $A54="geoshape", $A54="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="216" priority="125" stopIfTrue="1">
-      <formula>OR($A54="audio audit", $A54="text audit", $A54="speed violations count", $A54="speed violations list", $A54="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="215" priority="126" stopIfTrue="1">
-      <formula>OR($A54="username", $A54="phonenumber", $A54="start", $A54="end", $A54="deviceid", $A54="subscriberid", $A54="simserial", $A54="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="214" priority="128" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A54, 16)="select_multiple ", LEN($A54)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A54, 17)))), AND(LEFT($A54, 11)="select_one ", LEN($A54)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A54, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="213" priority="130" stopIfTrue="1">
-      <formula>$A54="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="212" priority="132" stopIfTrue="1">
-      <formula>$A54="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="211" priority="134" stopIfTrue="1">
-      <formula>$A54="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="210" priority="135" stopIfTrue="1">
-      <formula>$A54="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="209" priority="137" stopIfTrue="1">
-      <formula>$A54="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="208" priority="138" stopIfTrue="1">
-      <formula>$A54="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="207" priority="140" stopIfTrue="1">
-      <formula>$A54="begin group"</formula>
+  <conditionalFormatting sqref="A53:W53">
+    <cfRule type="expression" dxfId="190" priority="107" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A53, 14)="sensor_stream ", LEN($A53)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A53, 15)))), AND(LEFT($A53, 17)="sensor_statistic ", LEN($A53)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A53, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="189" priority="109" stopIfTrue="1">
+      <formula>$A53="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="188" priority="111" stopIfTrue="1">
+      <formula>OR($A53="audio", $A53="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="187" priority="113" stopIfTrue="1">
+      <formula>$A53="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="186" priority="115" stopIfTrue="1">
+      <formula>OR($A53="date", $A53="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="185" priority="117" stopIfTrue="1">
+      <formula>OR($A53="calculate", $A53="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="119" stopIfTrue="1">
+      <formula>$A53="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="183" priority="121" stopIfTrue="1">
+      <formula>$A53="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="182" priority="123" stopIfTrue="1">
+      <formula>OR($A53="geopoint", $A53="geoshape", $A53="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="181" priority="125" stopIfTrue="1">
+      <formula>OR($A53="audio audit", $A53="text audit", $A53="speed violations count", $A53="speed violations list", $A53="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="180" priority="126" stopIfTrue="1">
+      <formula>OR($A53="username", $A53="phonenumber", $A53="start", $A53="end", $A53="deviceid", $A53="subscriberid", $A53="simserial", $A53="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="179" priority="128" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A53, 16)="select_multiple ", LEN($A53)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A53, 17)))), AND(LEFT($A53, 11)="select_one ", LEN($A53)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A53, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="178" priority="130" stopIfTrue="1">
+      <formula>$A53="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="177" priority="132" stopIfTrue="1">
+      <formula>$A53="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="176" priority="134" stopIfTrue="1">
+      <formula>$A53="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="175" priority="135" stopIfTrue="1">
+      <formula>$A53="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="137" stopIfTrue="1">
+      <formula>$A53="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="173" priority="138" stopIfTrue="1">
+      <formula>$A53="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="140" stopIfTrue="1">
+      <formula>$A53="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="206" priority="108" stopIfTrue="1">
-      <formula>$A54="comments"</formula>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" dxfId="171" priority="108" stopIfTrue="1">
+      <formula>$A53="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54 F54">
-    <cfRule type="expression" dxfId="205" priority="106" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A54, 14)="sensor_stream ", LEN($A54)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A54, 15)))), AND(LEFT($A54, 17)="sensor_statistic ", LEN($A54)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A54, 18)))))</formula>
+  <conditionalFormatting sqref="B53 F53">
+    <cfRule type="expression" dxfId="170" priority="106" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A53, 14)="sensor_stream ", LEN($A53)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A53, 15)))), AND(LEFT($A53, 17)="sensor_statistic ", LEN($A53)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A53, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I34 B32:C34 F32:F34">
-    <cfRule type="expression" dxfId="204" priority="104" stopIfTrue="1">
-      <formula>$A32="begin group"</formula>
+  <conditionalFormatting sqref="I31:I33 B31:C33 F31:F33">
+    <cfRule type="expression" dxfId="169" priority="104" stopIfTrue="1">
+      <formula>$A31="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I34 B32:C34 O32:O34">
-    <cfRule type="expression" dxfId="203" priority="101" stopIfTrue="1">
-      <formula>$A32="begin repeat"</formula>
+  <conditionalFormatting sqref="I31:I33 B31:C33 O31:O33">
+    <cfRule type="expression" dxfId="168" priority="101" stopIfTrue="1">
+      <formula>$A31="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:D34 F32:F34">
-    <cfRule type="expression" dxfId="202" priority="98" stopIfTrue="1">
-      <formula>$A32="text"</formula>
+  <conditionalFormatting sqref="B31:D33 F31:F33">
+    <cfRule type="expression" dxfId="167" priority="98" stopIfTrue="1">
+      <formula>$A31="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32:H34 B32:D34">
-    <cfRule type="expression" dxfId="201" priority="96" stopIfTrue="1">
-      <formula>$A32="integer"</formula>
+  <conditionalFormatting sqref="G31:H33 B31:D33">
+    <cfRule type="expression" dxfId="166" priority="96" stopIfTrue="1">
+      <formula>$A31="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32:H34 B32:D34">
-    <cfRule type="expression" dxfId="200" priority="94" stopIfTrue="1">
-      <formula>$A32="decimal"</formula>
+  <conditionalFormatting sqref="G31:H33 B31:D33">
+    <cfRule type="expression" dxfId="165" priority="94" stopIfTrue="1">
+      <formula>$A31="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:C34 F32:F34">
-    <cfRule type="expression" dxfId="199" priority="92" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A32, 16)="select_multiple ", LEN($A32)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A32, 17)))), AND(LEFT($A32, 11)="select_one ", LEN($A32)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A32, 12)))))</formula>
+  <conditionalFormatting sqref="B31:C33 F31:F33">
+    <cfRule type="expression" dxfId="164" priority="92" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A31, 16)="select_multiple ", LEN($A31)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A31, 17)))), AND(LEFT($A31, 11)="select_one ", LEN($A31)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A31, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B34 F32:F34">
-    <cfRule type="expression" dxfId="198" priority="89" stopIfTrue="1">
-      <formula>OR($A32="audio audit", $A32="text audit", $A32="speed violations count", $A32="speed violations list", $A32="speed violations audit")</formula>
+  <conditionalFormatting sqref="B31:B33 F31:F33">
+    <cfRule type="expression" dxfId="163" priority="89" stopIfTrue="1">
+      <formula>OR($A31="audio audit", $A31="text audit", $A31="speed violations count", $A31="speed violations list", $A31="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:C34">
-    <cfRule type="expression" dxfId="197" priority="83" stopIfTrue="1">
-      <formula>$A32="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="196" priority="85" stopIfTrue="1">
-      <formula>$A32="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="195" priority="87" stopIfTrue="1">
-      <formula>OR($A32="geopoint", $A32="geoshape", $A32="geotrace")</formula>
+  <conditionalFormatting sqref="B31:C33">
+    <cfRule type="expression" dxfId="162" priority="83" stopIfTrue="1">
+      <formula>$A31="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="161" priority="85" stopIfTrue="1">
+      <formula>$A31="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="87" stopIfTrue="1">
+      <formula>OR($A31="geopoint", $A31="geoshape", $A31="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B34 N32:N34">
-    <cfRule type="expression" dxfId="194" priority="81" stopIfTrue="1">
-      <formula>OR($A32="calculate", $A32="calculate_here")</formula>
+  <conditionalFormatting sqref="B31:B33 N31:N33">
+    <cfRule type="expression" dxfId="159" priority="81" stopIfTrue="1">
+      <formula>OR($A31="calculate", $A31="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:C34 F32:F34">
-    <cfRule type="expression" dxfId="193" priority="79" stopIfTrue="1">
-      <formula>OR($A32="date", $A32="datetime")</formula>
+  <conditionalFormatting sqref="B31:C33 F31:F33">
+    <cfRule type="expression" dxfId="158" priority="79" stopIfTrue="1">
+      <formula>OR($A31="date", $A31="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:C34 F32:F34">
-    <cfRule type="expression" dxfId="192" priority="77" stopIfTrue="1">
-      <formula>$A32="image"</formula>
+  <conditionalFormatting sqref="B31:C33 F31:F33">
+    <cfRule type="expression" dxfId="157" priority="77" stopIfTrue="1">
+      <formula>$A31="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:C34">
-    <cfRule type="expression" dxfId="191" priority="75" stopIfTrue="1">
-      <formula>OR($A32="audio", $A32="video")</formula>
+  <conditionalFormatting sqref="B31:C33">
+    <cfRule type="expression" dxfId="156" priority="75" stopIfTrue="1">
+      <formula>OR($A31="audio", $A31="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32:W34">
-    <cfRule type="expression" dxfId="190" priority="72" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A32, 14)="sensor_stream ", LEN($A32)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A32, 15)))), AND(LEFT($A32, 17)="sensor_statistic ", LEN($A32)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A32, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="189" priority="74" stopIfTrue="1">
-      <formula>$A32="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="188" priority="76" stopIfTrue="1">
-      <formula>OR($A32="audio", $A32="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="187" priority="78" stopIfTrue="1">
-      <formula>$A32="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="186" priority="80" stopIfTrue="1">
-      <formula>OR($A32="date", $A32="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="185" priority="82" stopIfTrue="1">
-      <formula>OR($A32="calculate", $A32="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="184" priority="84" stopIfTrue="1">
-      <formula>$A32="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="86" stopIfTrue="1">
-      <formula>$A32="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="88" stopIfTrue="1">
-      <formula>OR($A32="geopoint", $A32="geoshape", $A32="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="181" priority="90" stopIfTrue="1">
-      <formula>OR($A32="audio audit", $A32="text audit", $A32="speed violations count", $A32="speed violations list", $A32="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>OR($A32="username", $A32="phonenumber", $A32="start", $A32="end", $A32="deviceid", $A32="subscriberid", $A32="simserial", $A32="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="179" priority="93" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A32, 16)="select_multiple ", LEN($A32)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A32, 17)))), AND(LEFT($A32, 11)="select_one ", LEN($A32)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A32, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="178" priority="95" stopIfTrue="1">
-      <formula>$A32="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="177" priority="97" stopIfTrue="1">
-      <formula>$A32="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="176" priority="99" stopIfTrue="1">
-      <formula>$A32="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="175" priority="100" stopIfTrue="1">
-      <formula>$A32="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="174" priority="102" stopIfTrue="1">
-      <formula>$A32="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="173" priority="103" stopIfTrue="1">
-      <formula>$A32="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="105" stopIfTrue="1">
-      <formula>$A32="begin group"</formula>
+  <conditionalFormatting sqref="A31:W33">
+    <cfRule type="expression" dxfId="155" priority="72" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A31, 14)="sensor_stream ", LEN($A31)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A31, 15)))), AND(LEFT($A31, 17)="sensor_statistic ", LEN($A31)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A31, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="74" stopIfTrue="1">
+      <formula>$A31="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="76" stopIfTrue="1">
+      <formula>OR($A31="audio", $A31="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="78" stopIfTrue="1">
+      <formula>$A31="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="151" priority="80" stopIfTrue="1">
+      <formula>OR($A31="date", $A31="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="82" stopIfTrue="1">
+      <formula>OR($A31="calculate", $A31="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="84" stopIfTrue="1">
+      <formula>$A31="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="86" stopIfTrue="1">
+      <formula>$A31="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="88" stopIfTrue="1">
+      <formula>OR($A31="geopoint", $A31="geoshape", $A31="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="90" stopIfTrue="1">
+      <formula>OR($A31="audio audit", $A31="text audit", $A31="speed violations count", $A31="speed violations list", $A31="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="91" stopIfTrue="1">
+      <formula>OR($A31="username", $A31="phonenumber", $A31="start", $A31="end", $A31="deviceid", $A31="subscriberid", $A31="simserial", $A31="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="93" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A31, 16)="select_multiple ", LEN($A31)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A31, 17)))), AND(LEFT($A31, 11)="select_one ", LEN($A31)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A31, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="95" stopIfTrue="1">
+      <formula>$A31="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="97" stopIfTrue="1">
+      <formula>$A31="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="99" stopIfTrue="1">
+      <formula>$A31="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="100" stopIfTrue="1">
+      <formula>$A31="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="102" stopIfTrue="1">
+      <formula>$A31="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="103" stopIfTrue="1">
+      <formula>$A31="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="105" stopIfTrue="1">
+      <formula>$A31="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B34">
-    <cfRule type="expression" dxfId="171" priority="73" stopIfTrue="1">
-      <formula>$A32="comments"</formula>
+  <conditionalFormatting sqref="B31:B33">
+    <cfRule type="expression" dxfId="136" priority="73" stopIfTrue="1">
+      <formula>$A31="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B34 F32:F34">
-    <cfRule type="expression" dxfId="170" priority="71" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A32, 14)="sensor_stream ", LEN($A32)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A32, 15)))), AND(LEFT($A32, 17)="sensor_statistic ", LEN($A32)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A32, 18)))))</formula>
+  <conditionalFormatting sqref="B31:B33 F31:F33">
+    <cfRule type="expression" dxfId="135" priority="71" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A31, 14)="sensor_stream ", LEN($A31)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A31, 15)))), AND(LEFT($A31, 17)="sensor_statistic ", LEN($A31)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A31, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:I46 B44:C46 F44:F46">
-    <cfRule type="expression" dxfId="169" priority="69" stopIfTrue="1">
-      <formula>$A44="begin group"</formula>
+  <conditionalFormatting sqref="I43:I45 B43:C45 F43:F45">
+    <cfRule type="expression" dxfId="134" priority="69" stopIfTrue="1">
+      <formula>$A43="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:I46 B44:C46 O44:O46">
-    <cfRule type="expression" dxfId="168" priority="66" stopIfTrue="1">
-      <formula>$A44="begin repeat"</formula>
+  <conditionalFormatting sqref="I43:I45 B43:C45 O43:O45">
+    <cfRule type="expression" dxfId="133" priority="66" stopIfTrue="1">
+      <formula>$A43="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:D46 F44:F46">
-    <cfRule type="expression" dxfId="167" priority="63" stopIfTrue="1">
-      <formula>$A44="text"</formula>
+  <conditionalFormatting sqref="B43:D45 F43:F45">
+    <cfRule type="expression" dxfId="132" priority="63" stopIfTrue="1">
+      <formula>$A43="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44:H46 B44:D46">
-    <cfRule type="expression" dxfId="166" priority="61" stopIfTrue="1">
-      <formula>$A44="integer"</formula>
+  <conditionalFormatting sqref="G43:H45 B43:D45">
+    <cfRule type="expression" dxfId="131" priority="61" stopIfTrue="1">
+      <formula>$A43="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44:H46 B44:D46">
-    <cfRule type="expression" dxfId="165" priority="59" stopIfTrue="1">
-      <formula>$A44="decimal"</formula>
+  <conditionalFormatting sqref="G43:H45 B43:D45">
+    <cfRule type="expression" dxfId="130" priority="59" stopIfTrue="1">
+      <formula>$A43="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:C46 F44:F46">
-    <cfRule type="expression" dxfId="164" priority="57" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A44, 16)="select_multiple ", LEN($A44)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A44, 17)))), AND(LEFT($A44, 11)="select_one ", LEN($A44)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A44, 12)))))</formula>
+  <conditionalFormatting sqref="B43:C45 F43:F45">
+    <cfRule type="expression" dxfId="129" priority="57" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A43, 16)="select_multiple ", LEN($A43)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A43, 17)))), AND(LEFT($A43, 11)="select_one ", LEN($A43)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A43, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:B46 F44:F46">
-    <cfRule type="expression" dxfId="163" priority="54" stopIfTrue="1">
-      <formula>OR($A44="audio audit", $A44="text audit", $A44="speed violations count", $A44="speed violations list", $A44="speed violations audit")</formula>
+  <conditionalFormatting sqref="B43:B45 F43:F45">
+    <cfRule type="expression" dxfId="128" priority="54" stopIfTrue="1">
+      <formula>OR($A43="audio audit", $A43="text audit", $A43="speed violations count", $A43="speed violations list", $A43="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:C46">
-    <cfRule type="expression" dxfId="162" priority="48" stopIfTrue="1">
-      <formula>$A44="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="161" priority="50" stopIfTrue="1">
-      <formula>$A44="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="52" stopIfTrue="1">
-      <formula>OR($A44="geopoint", $A44="geoshape", $A44="geotrace")</formula>
+  <conditionalFormatting sqref="B43:C45">
+    <cfRule type="expression" dxfId="127" priority="48" stopIfTrue="1">
+      <formula>$A43="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="50" stopIfTrue="1">
+      <formula>$A43="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="52" stopIfTrue="1">
+      <formula>OR($A43="geopoint", $A43="geoshape", $A43="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:B46 N44:N46">
-    <cfRule type="expression" dxfId="159" priority="46" stopIfTrue="1">
-      <formula>OR($A44="calculate", $A44="calculate_here")</formula>
+  <conditionalFormatting sqref="B43:B45 N43:N45">
+    <cfRule type="expression" dxfId="124" priority="46" stopIfTrue="1">
+      <formula>OR($A43="calculate", $A43="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:C46 F44:F46">
-    <cfRule type="expression" dxfId="158" priority="44" stopIfTrue="1">
-      <formula>OR($A44="date", $A44="datetime")</formula>
+  <conditionalFormatting sqref="B43:C45 F43:F45">
+    <cfRule type="expression" dxfId="123" priority="44" stopIfTrue="1">
+      <formula>OR($A43="date", $A43="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:C46 F44:F46">
-    <cfRule type="expression" dxfId="157" priority="42" stopIfTrue="1">
-      <formula>$A44="image"</formula>
+  <conditionalFormatting sqref="B43:C45 F43:F45">
+    <cfRule type="expression" dxfId="122" priority="42" stopIfTrue="1">
+      <formula>$A43="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:C46">
-    <cfRule type="expression" dxfId="156" priority="40" stopIfTrue="1">
-      <formula>OR($A44="audio", $A44="video")</formula>
+  <conditionalFormatting sqref="B43:C45">
+    <cfRule type="expression" dxfId="121" priority="40" stopIfTrue="1">
+      <formula>OR($A43="audio", $A43="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44:W46">
-    <cfRule type="expression" dxfId="155" priority="37" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A44, 14)="sensor_stream ", LEN($A44)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A44, 15)))), AND(LEFT($A44, 17)="sensor_statistic ", LEN($A44)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A44, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="39" stopIfTrue="1">
-      <formula>$A44="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="153" priority="41" stopIfTrue="1">
-      <formula>OR($A44="audio", $A44="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="152" priority="43" stopIfTrue="1">
-      <formula>$A44="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="151" priority="45" stopIfTrue="1">
-      <formula>OR($A44="date", $A44="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="47" stopIfTrue="1">
-      <formula>OR($A44="calculate", $A44="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="149" priority="49" stopIfTrue="1">
-      <formula>$A44="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>$A44="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="147" priority="53" stopIfTrue="1">
-      <formula>OR($A44="geopoint", $A44="geoshape", $A44="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="146" priority="55" stopIfTrue="1">
-      <formula>OR($A44="audio audit", $A44="text audit", $A44="speed violations count", $A44="speed violations list", $A44="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="56" stopIfTrue="1">
-      <formula>OR($A44="username", $A44="phonenumber", $A44="start", $A44="end", $A44="deviceid", $A44="subscriberid", $A44="simserial", $A44="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="144" priority="58" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A44, 16)="select_multiple ", LEN($A44)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A44, 17)))), AND(LEFT($A44, 11)="select_one ", LEN($A44)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A44, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="143" priority="60" stopIfTrue="1">
-      <formula>$A44="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="62" stopIfTrue="1">
-      <formula>$A44="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="64" stopIfTrue="1">
-      <formula>$A44="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="65" stopIfTrue="1">
-      <formula>$A44="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="67" stopIfTrue="1">
-      <formula>$A44="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="68" stopIfTrue="1">
-      <formula>$A44="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="70" stopIfTrue="1">
-      <formula>$A44="begin group"</formula>
+  <conditionalFormatting sqref="A43:W45">
+    <cfRule type="expression" dxfId="120" priority="37" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A43, 14)="sensor_stream ", LEN($A43)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A43, 15)))), AND(LEFT($A43, 17)="sensor_statistic ", LEN($A43)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A43, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="119" priority="39" stopIfTrue="1">
+      <formula>$A43="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="41" stopIfTrue="1">
+      <formula>OR($A43="audio", $A43="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="43" stopIfTrue="1">
+      <formula>$A43="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="45" stopIfTrue="1">
+      <formula>OR($A43="date", $A43="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="47" stopIfTrue="1">
+      <formula>OR($A43="calculate", $A43="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="49" stopIfTrue="1">
+      <formula>$A43="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="51" stopIfTrue="1">
+      <formula>$A43="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="53" stopIfTrue="1">
+      <formula>OR($A43="geopoint", $A43="geoshape", $A43="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="55" stopIfTrue="1">
+      <formula>OR($A43="audio audit", $A43="text audit", $A43="speed violations count", $A43="speed violations list", $A43="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="56" stopIfTrue="1">
+      <formula>OR($A43="username", $A43="phonenumber", $A43="start", $A43="end", $A43="deviceid", $A43="subscriberid", $A43="simserial", $A43="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="58" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A43, 16)="select_multiple ", LEN($A43)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A43, 17)))), AND(LEFT($A43, 11)="select_one ", LEN($A43)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A43, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="60" stopIfTrue="1">
+      <formula>$A43="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="62" stopIfTrue="1">
+      <formula>$A43="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="64" stopIfTrue="1">
+      <formula>$A43="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="65" stopIfTrue="1">
+      <formula>$A43="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="67" stopIfTrue="1">
+      <formula>$A43="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="68" stopIfTrue="1">
+      <formula>$A43="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="70" stopIfTrue="1">
+      <formula>$A43="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:B46">
-    <cfRule type="expression" dxfId="136" priority="38" stopIfTrue="1">
-      <formula>$A44="comments"</formula>
+  <conditionalFormatting sqref="B43:B45">
+    <cfRule type="expression" dxfId="101" priority="38" stopIfTrue="1">
+      <formula>$A43="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:B46 F44:F46">
-    <cfRule type="expression" dxfId="135" priority="36" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A44, 14)="sensor_stream ", LEN($A44)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A44, 15)))), AND(LEFT($A44, 17)="sensor_statistic ", LEN($A44)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A44, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I56:I58 B56:C58 F56:F58">
-    <cfRule type="expression" dxfId="134" priority="34" stopIfTrue="1">
-      <formula>$A56="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I56:I58 B56:C58">
-    <cfRule type="expression" dxfId="133" priority="31" stopIfTrue="1">
-      <formula>$A56="begin repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:D58 F56:F58">
-    <cfRule type="expression" dxfId="132" priority="28" stopIfTrue="1">
-      <formula>$A56="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56:H58 B56:D58">
-    <cfRule type="expression" dxfId="131" priority="26" stopIfTrue="1">
-      <formula>$A56="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56:H58 B56:D58">
-    <cfRule type="expression" dxfId="130" priority="24" stopIfTrue="1">
-      <formula>$A56="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:C58 F56:F58">
-    <cfRule type="expression" dxfId="129" priority="22" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A56, 16)="select_multiple ", LEN($A56)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A56, 17)))), AND(LEFT($A56, 11)="select_one ", LEN($A56)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A56, 12)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:B58 F56:F58">
-    <cfRule type="expression" dxfId="128" priority="19" stopIfTrue="1">
-      <formula>OR($A56="audio audit", $A56="text audit", $A56="speed violations count", $A56="speed violations list", $A56="speed violations audit")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:C58">
-    <cfRule type="expression" dxfId="127" priority="13" stopIfTrue="1">
-      <formula>$A56="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
-      <formula>$A56="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="17" stopIfTrue="1">
-      <formula>OR($A56="geopoint", $A56="geoshape", $A56="geotrace")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:B58 N56:N58">
-    <cfRule type="expression" dxfId="124" priority="11" stopIfTrue="1">
-      <formula>OR($A56="calculate", $A56="calculate_here")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:C58 F56:F58">
-    <cfRule type="expression" dxfId="123" priority="9" stopIfTrue="1">
-      <formula>OR($A56="date", $A56="datetime")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:C58 F56:F58">
-    <cfRule type="expression" dxfId="122" priority="7" stopIfTrue="1">
-      <formula>$A56="image"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:C58">
-    <cfRule type="expression" dxfId="121" priority="5" stopIfTrue="1">
-      <formula>OR($A56="audio", $A56="video")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:N58">
-    <cfRule type="expression" dxfId="120" priority="2" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A56, 14)="sensor_stream ", LEN($A56)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A56, 15)))), AND(LEFT($A56, 17)="sensor_statistic ", LEN($A56)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A56, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="4" stopIfTrue="1">
-      <formula>$A56="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="6" stopIfTrue="1">
-      <formula>OR($A56="audio", $A56="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="8" stopIfTrue="1">
-      <formula>$A56="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="10" stopIfTrue="1">
-      <formula>OR($A56="date", $A56="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="12" stopIfTrue="1">
-      <formula>OR($A56="calculate", $A56="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="14" stopIfTrue="1">
-      <formula>$A56="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>$A56="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="18" stopIfTrue="1">
-      <formula>OR($A56="geopoint", $A56="geoshape", $A56="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="20" stopIfTrue="1">
-      <formula>OR($A56="audio audit", $A56="text audit", $A56="speed violations count", $A56="speed violations list", $A56="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="21" stopIfTrue="1">
-      <formula>OR($A56="username", $A56="phonenumber", $A56="start", $A56="end", $A56="deviceid", $A56="subscriberid", $A56="simserial", $A56="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="23" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A56, 16)="select_multiple ", LEN($A56)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A56, 17)))), AND(LEFT($A56, 11)="select_one ", LEN($A56)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A56, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="25" stopIfTrue="1">
-      <formula>$A56="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="27" stopIfTrue="1">
-      <formula>$A56="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="29" stopIfTrue="1">
-      <formula>$A56="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="30" stopIfTrue="1">
-      <formula>$A56="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="32" stopIfTrue="1">
-      <formula>$A56="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="33" stopIfTrue="1">
-      <formula>$A56="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="35" stopIfTrue="1">
-      <formula>$A56="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:B58">
-    <cfRule type="expression" dxfId="101" priority="3" stopIfTrue="1">
-      <formula>$A56="comments"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:B58 F56:F58">
-    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A56, 14)="sensor_stream ", LEN($A56)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A56, 15)))), AND(LEFT($A56, 17)="sensor_statistic ", LEN($A56)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A56, 18)))))</formula>
+  <conditionalFormatting sqref="B43:B45 F43:F45">
+    <cfRule type="expression" dxfId="100" priority="36" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A43, 14)="sensor_stream ", LEN($A43)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A43, 15)))), AND(LEFT($A43, 17)="sensor_statistic ", LEN($A43)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A43, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -8333,7 +7857,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007232029</v>
+        <v>2007301658</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>369</v>
@@ -8925,7 +8449,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>

</xml_diff>